<commit_message>
ajustes nos conflitos após o merge das versões rotina e olympics
</commit_message>
<xml_diff>
--- a/scripts/String_21_06_2016.xlsx
+++ b/scripts/String_21_06_2016.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6276" uniqueCount="5773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6283" uniqueCount="5780">
   <si>
     <t>Português</t>
   </si>
@@ -17339,6 +17339,27 @@
   </si>
   <si>
     <t>Joignez-vous Gardiens de la santé de demain pour jouer à nouveau</t>
+  </si>
+  <si>
+    <t>Resposta CORRETA!</t>
+  </si>
+  <si>
+    <t>Right answer!</t>
+  </si>
+  <si>
+    <t>Respuesta adecuada!</t>
+  </si>
+  <si>
+    <t>合適的回答！</t>
+  </si>
+  <si>
+    <t>الجواب الصحيح!</t>
+  </si>
+  <si>
+    <t>Нужное!</t>
+  </si>
+  <si>
+    <t>Bonne réponse!</t>
   </si>
 </sst>
 </file>
@@ -17874,8 +17895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B891" workbookViewId="0">
-      <selection activeCell="D891" sqref="D891"/>
+    <sheetView tabSelected="1" topLeftCell="A891" workbookViewId="0">
+      <selection activeCell="F897" sqref="F897"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
@@ -55617,13 +55638,27 @@
       <c r="Z898" s="2"/>
     </row>
     <row r="899" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A899" s="2"/>
-      <c r="B899" s="2"/>
-      <c r="C899" s="2"/>
-      <c r="D899" s="2"/>
-      <c r="E899" s="2"/>
-      <c r="F899" s="2"/>
-      <c r="G899" s="2"/>
+      <c r="A899" s="2" t="s">
+        <v>5773</v>
+      </c>
+      <c r="B899" s="2" t="s">
+        <v>5774</v>
+      </c>
+      <c r="C899" s="2" t="s">
+        <v>5775</v>
+      </c>
+      <c r="D899" s="2" t="s">
+        <v>5776</v>
+      </c>
+      <c r="E899" s="2" t="s">
+        <v>5777</v>
+      </c>
+      <c r="F899" s="2" t="s">
+        <v>5778</v>
+      </c>
+      <c r="G899" s="2" t="s">
+        <v>5779</v>
+      </c>
       <c r="H899" s="2"/>
       <c r="I899" s="2"/>
       <c r="J899" s="2"/>

</xml_diff>